<commit_message>
Update 11/08/2022 : datapaper
</commit_message>
<xml_diff>
--- a/data/FSM.xlsx
+++ b/data/FSM.xlsx
@@ -32,12 +32,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>Sexe</t>
-  </si>
-  <si>
-    <t>Fishbase</t>
-  </si>
-  <si>
     <t>Chelidonichthys cuculus</t>
   </si>
   <si>
@@ -345,6 +339,12 @@
   </si>
   <si>
     <t>Sparisoma viride</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>FSM</t>
   </si>
 </sst>
 </file>
@@ -739,7 +739,7 @@
   <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,1518 +752,1518 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="str">
         <f t="shared" ref="B2:B11" si="0">A2</f>
         <v>Chelidonichthys cuculus</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Chelidonichthys cuculus</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Clupea clupea</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Clupea clupea</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="str">
         <f>A6</f>
         <v>Dicentrarchus labrax</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" ref="B7:B9" si="1">A7</f>
         <v>Dicentrarchus labrax</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Argyrosomus regius</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Argyrosomus regius</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Engraulis encrasicolus</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Engraulis encrasicolus</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="str">
         <f t="shared" ref="B16:B29" si="2">A16</f>
         <v>Merluccius merluccius</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Merluccius merluccius</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Mullus surmuletus</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Mullus surmuletus</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Pagellus bogaraveo</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Pagellus bogaraveo</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Scomber scombrus</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Scomber scombrus</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Solea solea</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Solea solea</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Sprattus sprattus</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B27" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Sprattus sprattus</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Sardina pilchardus</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Sardina pilchardus</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 17/08/2022 : datapaper
</commit_message>
<xml_diff>
--- a/data/FSM.xlsx
+++ b/data/FSM.xlsx
@@ -738,11 +738,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Update 09/09/2022 : New photos update
</commit_message>
<xml_diff>
--- a/data/FSM.xlsx
+++ b/data/FSM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="114">
   <si>
     <t>SubSpecies</t>
   </si>
@@ -345,6 +345,27 @@
   </si>
   <si>
     <t>FSM</t>
+  </si>
+  <si>
+    <t>Acanthostracion sp.</t>
+  </si>
+  <si>
+    <t>Acanthurus sp.</t>
+  </si>
+  <si>
+    <t>Acanthostracion quadricornis</t>
+  </si>
+  <si>
+    <t>Acanthurus chirurgus</t>
+  </si>
+  <si>
+    <t>Caranx bartholomaei</t>
+  </si>
+  <si>
+    <t>Seriola rivoliana</t>
+  </si>
+  <si>
+    <t>Anisotremus surinamensis</t>
   </si>
 </sst>
 </file>
@@ -736,15 +757,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1406,7 +1428,7 @@
         <v>69</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>3</v>
@@ -1420,7 +1442,7 @@
         <v>69</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>5</v>
@@ -1431,10 +1453,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>3</v>
@@ -1445,10 +1467,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>5</v>
@@ -1459,10 +1481,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>3</v>
@@ -1473,10 +1495,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>5</v>
@@ -1487,10 +1509,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>3</v>
@@ -1501,10 +1523,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>5</v>
@@ -1515,10 +1537,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>3</v>
@@ -1529,10 +1551,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>5</v>
@@ -1543,10 +1565,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>3</v>
@@ -1557,10 +1579,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>5</v>
@@ -1571,10 +1593,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>3</v>
@@ -1585,10 +1607,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>5</v>
@@ -1599,10 +1621,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>3</v>
@@ -1613,10 +1635,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>5</v>
@@ -1627,10 +1649,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>3</v>
@@ -1641,10 +1663,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>5</v>
@@ -1655,10 +1677,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>3</v>
@@ -1669,10 +1691,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>5</v>
@@ -1683,10 +1705,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>3</v>
@@ -1697,10 +1719,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>5</v>
@@ -1711,10 +1733,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>3</v>
@@ -1725,10 +1747,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>5</v>
@@ -1739,10 +1761,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>3</v>
@@ -1753,10 +1775,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>5</v>
@@ -1767,10 +1789,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>3</v>
@@ -1781,10 +1803,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>5</v>
@@ -1795,10 +1817,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>3</v>
@@ -1809,10 +1831,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>5</v>
@@ -1823,10 +1845,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>3</v>
@@ -1837,10 +1859,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>5</v>
@@ -1851,7 +1873,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>85</v>
@@ -1865,7 +1887,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>85</v>
@@ -1879,7 +1901,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>85</v>
@@ -1893,7 +1915,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>85</v>
@@ -1907,10 +1929,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>3</v>
@@ -1921,10 +1943,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>5</v>
@@ -1935,10 +1957,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>3</v>
@@ -1949,10 +1971,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>5</v>
@@ -1963,10 +1985,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>3</v>
@@ -1977,10 +1999,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>5</v>
@@ -1991,7 +2013,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>91</v>
@@ -2005,7 +2027,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>91</v>
@@ -2019,10 +2041,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>3</v>
@@ -2033,10 +2055,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>5</v>
@@ -2047,10 +2069,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>3</v>
@@ -2061,10 +2083,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>5</v>
@@ -2075,10 +2097,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>3</v>
@@ -2089,10 +2111,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>5</v>
@@ -2103,10 +2125,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>3</v>
@@ -2117,10 +2139,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>5</v>
@@ -2131,10 +2153,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>3</v>
@@ -2145,10 +2167,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>5</v>
@@ -2159,10 +2181,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>3</v>
@@ -2173,10 +2195,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>5</v>
@@ -2187,10 +2209,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>3</v>
@@ -2201,10 +2223,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>5</v>
@@ -2215,10 +2237,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>3</v>
@@ -2229,10 +2251,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>5</v>
@@ -2243,7 +2265,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>101</v>
@@ -2257,7 +2279,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>101</v>
@@ -2266,6 +2288,146 @@
         <v>5</v>
       </c>
       <c r="D107" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117" s="4" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update 07/07/2023 : MED files
</commit_message>
<xml_diff>
--- a/data/FSM.xlsx
+++ b/data/FSM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alemeled\Desktop\GitHub Mat\MaturityScaleTools\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alemeled\Desktop\GitHubMATURITY\MaturityScaleTools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="123">
   <si>
     <t>SubSpecies</t>
   </si>
@@ -366,6 +366,33 @@
   </si>
   <si>
     <t>Anisotremus surinamensis</t>
+  </si>
+  <si>
+    <t>Mullus sp.</t>
+  </si>
+  <si>
+    <t>Trisopterus minutus</t>
+  </si>
+  <si>
+    <t>Trachurus trachurus</t>
+  </si>
+  <si>
+    <t>Trachurus sp.</t>
+  </si>
+  <si>
+    <t>Trachurus mediterraneus</t>
+  </si>
+  <si>
+    <t>Eutrigla gurnardus</t>
+  </si>
+  <si>
+    <t>Sparus aurata</t>
+  </si>
+  <si>
+    <t>Boops boops</t>
+  </si>
+  <si>
+    <t>Mullus barbatus</t>
   </si>
 </sst>
 </file>
@@ -451,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -475,6 +502,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -757,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,9 +1053,8 @@
       <c r="A18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Mullus surmuletus</v>
+      <c r="B18" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>3</v>
@@ -1038,9 +1067,8 @@
       <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Mullus surmuletus</v>
+      <c r="B19" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
@@ -2428,6 +2456,202 @@
         <v>5</v>
       </c>
       <c r="D117" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C126" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C127" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C128" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C130" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C131" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D131" s="4" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update 19/07/2023 : New file added
</commit_message>
<xml_diff>
--- a/data/FSM.xlsx
+++ b/data/FSM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="124">
   <si>
     <t>SubSpecies</t>
   </si>
@@ -393,6 +393,9 @@
   </si>
   <si>
     <t>Mullus barbatus</t>
+  </si>
+  <si>
+    <t>Osmerus eperlanus</t>
   </si>
 </sst>
 </file>
@@ -787,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+      <selection activeCell="A132" sqref="A132:D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,6 +2658,34 @@
         <v>33</v>
       </c>
     </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C132" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D132" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C133" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D133" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>